<commit_message>
PROS-6288 -  MOLSONCOORSHR - development
</commit_message>
<xml_diff>
--- a/Projects/MOLSONCOORSHR/Data/MOLSONCOORS_CE_KPIs.xlsx
+++ b/Projects/MOLSONCOORSHR/Data/MOLSONCOORS_CE_KPIs.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t xml:space="preserve">KPI name Eng</t>
   </si>
@@ -86,7 +86,7 @@
     <t xml:space="preserve">Score Function</t>
   </si>
   <si>
-    <t xml:space="preserve">Lower Thershold</t>
+    <t xml:space="preserve">Lower Threshold</t>
   </si>
   <si>
     <t xml:space="preserve">Higher Threshold</t>
@@ -101,7 +101,7 @@
     <t xml:space="preserve">Ambient</t>
   </si>
   <si>
-    <t xml:space="preserve">SOS vs Target</t>
+    <t xml:space="preserve">Linear SOS vs Target</t>
   </si>
   <si>
     <t xml:space="preserve">Weighted Score</t>
@@ -134,31 +134,10 @@
     <t xml:space="preserve">Cooler, Ambient</t>
   </si>
   <si>
+    <t xml:space="preserve">Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sum of Scores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOS Ambient 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOS 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOS Cooler 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facings Ambient 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facings 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facings Cooler 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distribution 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Store Score 2</t>
   </si>
 </sst>
 </file>
@@ -323,10 +302,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -336,6 +311,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -437,9 +416,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9360</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>349200</xdr:rowOff>
+      <xdr:colOff>9000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -449,7 +428,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="16151040" cy="9245520"/>
+          <a:ext cx="16887240" cy="7843320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -481,26 +460,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.5627530364372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.1336032388664"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.8461538461538"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="35.8502024291498"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="21.4251012145749"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.2753036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="44.8461538461538"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="37.4210526315789"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="22.4251012145749"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="20.8542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -549,19 +528,17 @@
       <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="9" t="n">
+      <c r="G2" s="8" t="n">
         <v>0.2</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="9" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J2" s="9" t="n">
+      <c r="I2" s="8"/>
+      <c r="J2" s="8" t="n">
         <v>0.8</v>
       </c>
       <c r="K2" s="0" t="n">
@@ -582,19 +559,17 @@
       <c r="E3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="9" t="n">
+      <c r="G3" s="8" t="n">
         <v>0.2</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="9" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="J3" s="9" t="n">
+      <c r="I3" s="8"/>
+      <c r="J3" s="8" t="n">
         <v>0.9</v>
       </c>
       <c r="K3" s="0" t="n">
@@ -605,7 +580,7 @@
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="4"/>
@@ -615,19 +590,17 @@
       <c r="E4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="9" t="n">
+      <c r="G4" s="8" t="n">
         <v>0.2</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="9" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="J4" s="9" t="n">
+      <c r="I4" s="8"/>
+      <c r="J4" s="8" t="n">
         <v>0.8</v>
       </c>
       <c r="K4" s="0" t="n">
@@ -638,7 +611,7 @@
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="4"/>
@@ -648,19 +621,17 @@
       <c r="E5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="8" t="n">
+      <c r="F5" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="9" t="n">
+      <c r="G5" s="8" t="n">
         <v>0.2</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="9" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="J5" s="9" t="n">
+      <c r="I5" s="8"/>
+      <c r="J5" s="8" t="n">
         <v>0.8</v>
       </c>
       <c r="K5" s="0" t="n">
@@ -668,32 +639,30 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="51.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="9" t="n">
+      <c r="G6" s="8" t="n">
         <v>0.2</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="9" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="J6" s="9" t="n">
+      <c r="I6" s="8"/>
+      <c r="J6" s="8" t="n">
         <v>0.8</v>
       </c>
       <c r="K6" s="0" t="n">
@@ -714,10 +683,10 @@
       <c r="E7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="12"/>
-      <c r="H7" s="8" t="s">
-        <v>14</v>
+      <c r="H7" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -732,17 +701,17 @@
       <c r="B8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="12"/>
-      <c r="H8" s="8" t="s">
-        <v>14</v>
+      <c r="H8" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
@@ -762,252 +731,14 @@
       <c r="E9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="7"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="8" t="s">
-        <v>14</v>
+      <c r="H9" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="0" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="51.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="9" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="9" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J10" s="9" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="51.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="9" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="9" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="J11" s="9" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="51.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="9" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="9" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="J12" s="9" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="51.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="9" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="9" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="J13" s="9" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="51.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="9" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="9" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="J14" s="9" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="51.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="51.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="51.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="0" t="n">
         <v>90</v>
       </c>
     </row>

</xml_diff>